<commit_message>
can read cash balance file and cash activity file now
</commit_message>
<xml_diff>
--- a/samples/Cash Stt _21042020.xlsx
+++ b/samples/Cash Stt _21042020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Reconciliation\JIC International\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\bochk_revised2\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{920CF0D8-3884-4005-993E-47535CF1086A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E613CF1-0729-4D07-A5D3-652AB3FD1F15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Account Balance" sheetId="1" r:id="rId1"/>
@@ -432,176 +432,176 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -1399,14 +1399,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="5" width="9.140625" style="2"/>
     <col min="6" max="7" width="11" style="2" bestFit="1" customWidth="1"/>
@@ -1416,7 +1416,7 @@
     <col min="13" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="107.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="87.75">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1471,10 +1471,10 @@
         <v>4</v>
       </c>
       <c r="F2" s="2">
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="G2" s="2">
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="H2" s="2">
         <v>0</v>
@@ -1492,7 +1492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1623,10 +1623,10 @@
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>0</v>
+        <v>456</v>
       </c>
       <c r="G6" s="2">
-        <v>0</v>
+        <v>456</v>
       </c>
       <c r="H6" s="2">
         <v>0</v>

</xml_diff>